<commit_message>
fix pb level_dafault_list, fix shapes in split_, EN style
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/split_few_bars.xlsx
+++ b/xlsx/country_comparison/split_few_bars.xlsx
@@ -445,8 +445,8 @@
       <c r="B2" t="n">
         <v>0.172543292244347</v>
       </c>
-      <c r="C2" t="e">
-        <v>#NUM!</v>
+      <c r="C2" t="n">
+        <v>0.208838632887556</v>
       </c>
       <c r="D2" t="n">
         <v>0.138840103970168</v>
@@ -486,8 +486,8 @@
       <c r="B3" t="n">
         <v>0.20922419214653</v>
       </c>
-      <c r="C3" t="e">
-        <v>#NUM!</v>
+      <c r="C3" t="n">
+        <v>0.178857494432493</v>
       </c>
       <c r="D3" t="n">
         <v>0.169560940391051</v>
@@ -527,8 +527,8 @@
       <c r="B4" t="n">
         <v>0.198876819805837</v>
       </c>
-      <c r="C4" t="e">
-        <v>#NUM!</v>
+      <c r="C4" t="n">
+        <v>0.187422136325044</v>
       </c>
       <c r="D4" t="n">
         <v>0.254402568967971</v>
@@ -568,8 +568,8 @@
       <c r="B5" t="n">
         <v>0.187225256109629</v>
       </c>
-      <c r="C5" t="e">
-        <v>#NUM!</v>
+      <c r="C5" t="n">
+        <v>0.188547853061829</v>
       </c>
       <c r="D5" t="n">
         <v>0.187734829873696</v>
@@ -609,8 +609,8 @@
       <c r="B6" t="n">
         <v>0.232130439693656</v>
       </c>
-      <c r="C6" t="e">
-        <v>#NUM!</v>
+      <c r="C6" t="n">
+        <v>0.236333883293078</v>
       </c>
       <c r="D6" t="n">
         <v>0.249461556797114</v>

</xml_diff>